<commit_message>
Add EventType Models, Views and Controller. Adding new EventTypes and Showing existing EventTypes implemented.
</commit_message>
<xml_diff>
--- a/EventManager/TODO.xlsx
+++ b/EventManager/TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
   <si>
     <t>Priority</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Eventtypes</t>
-  </si>
-  <si>
-    <t>Eventtype colors</t>
   </si>
   <si>
     <t>EventTime/Day</t>
@@ -218,6 +215,33 @@
   </si>
   <si>
     <t>Deprecated</t>
+  </si>
+  <si>
+    <t>FormatedEventtype</t>
+  </si>
+  <si>
+    <t>Add Formatting to EventType</t>
+  </si>
+  <si>
+    <t>Convert EventType to FormatedEventType</t>
+  </si>
+  <si>
+    <t>Add styles to EventItems which contain FormatedEventType</t>
+  </si>
+  <si>
+    <t>FormatedEventType ViewStyles</t>
+  </si>
+  <si>
+    <t>Add EventType to EventItem</t>
+  </si>
+  <si>
+    <t>Apply Type to an Event</t>
+  </si>
+  <si>
+    <t>ListView for existing EventTypes</t>
+  </si>
+  <si>
+    <t>Custom HtmlElement to visualize existing EventTypes</t>
   </si>
 </sst>
 </file>
@@ -349,7 +373,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -366,6 +390,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -375,7 +400,7 @@
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="68">
     <dxf>
       <font>
         <b/>
@@ -463,6 +488,53 @@
     </dxf>
     <dxf>
       <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color theme="0"/>
@@ -470,65 +542,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -547,6 +560,53 @@
     </dxf>
     <dxf>
       <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color theme="0"/>
@@ -563,6 +623,42 @@
         <i val="0"/>
         <color auto="1"/>
       </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
@@ -577,12 +673,122 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike/>
         <color theme="0"/>
       </font>
@@ -596,25 +802,137 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color auto="1"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
       <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike/>
         <color theme="0"/>
       </font>
@@ -626,6 +944,8 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -636,7 +956,9 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
@@ -646,6 +968,8 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -656,6 +980,8 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -666,27 +992,133 @@
     </dxf>
     <dxf>
       <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color auto="1"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
       <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
       <font>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -697,6 +1129,33 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -707,7 +1166,9 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
@@ -717,6 +1178,8 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -735,699 +1198,6 @@
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1435,14 +1205,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H30" totalsRowShown="0">
-  <sortState ref="A2:H30">
-    <sortCondition descending="1" ref="C2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H35" totalsRowShown="0">
+  <sortState ref="A2:H35">
+    <sortCondition descending="1" ref="C1"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Projectdependency _x000a_((low)1-(high)5)"/>
-    <tableColumn id="2" name="Effort _x000a_((low)1-(high)5)" dataDxfId="98"/>
-    <tableColumn id="8" name="Priority" dataDxfId="97">
+    <tableColumn id="2" name="Effort _x000a_((low)1-(high)5)" dataDxfId="55"/>
+    <tableColumn id="8" name="Priority" dataDxfId="54">
       <calculatedColumnFormula>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</calculatedColumnFormula>
@@ -1767,15 +1537,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
@@ -1786,10 +1556,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="27.75" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1801,13 +1571,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1824,17 +1594,17 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1851,13 +1621,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1874,16 +1644,16 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
         <v>63</v>
-      </c>
-      <c r="H4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1900,13 +1670,13 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1923,13 +1693,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1952,7 +1722,7 @@
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1969,13 +1739,13 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1995,18 +1765,18 @@
         <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <f>(Tabelle1[[#This Row],[Projectdependency 
@@ -2015,13 +1785,16 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2029,22 +1802,25 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2052,30 +1828,30 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="C12">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>(Tabelle1[[#This Row],[Projectdependency 
@@ -2084,22 +1860,22 @@
         <v>3.5</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
       <c r="C14">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
@@ -2107,13 +1883,13 @@
         <v>3.5</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2130,21 +1906,21 @@
         <v>3.5</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <f>(Tabelle1[[#This Row],[Projectdependency 
@@ -2153,62 +1929,59 @@
         <v>3.5</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
         <v>2</v>
       </c>
-      <c r="B17">
-        <v>1.5</v>
-      </c>
       <c r="C17">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2216,30 +1989,30 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C19">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <f>(Tabelle1[[#This Row],[Projectdependency 
@@ -2248,13 +2021,16 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2271,21 +2047,21 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <f>(Tabelle1[[#This Row],[Projectdependency 
@@ -2294,36 +2070,36 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
         <v>3</v>
       </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23">
-        <f>(Tabelle1[[#This Row],[Projectdependency 
-((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
-((low)1-(high)5)]]))/2</f>
-        <v>2.5</v>
-      </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2331,68 +2107,68 @@
         <v>2</v>
       </c>
       <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
         <v>3</v>
       </c>
-      <c r="C24">
-        <f>(Tabelle1[[#This Row],[Projectdependency 
-((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
-((low)1-(high)5)]]))/2</f>
-        <v>2.5</v>
-      </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="F24" t="s">
-        <v>62</v>
-      </c>
       <c r="H24" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
         <v>2.5</v>
       </c>
-      <c r="C25">
-        <f>(Tabelle1[[#This Row],[Projectdependency 
-((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
-((low)1-(high)5)]]))/2</f>
-        <v>2.25</v>
-      </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
         <v>4</v>
       </c>
-      <c r="C26">
-        <f>(Tabelle1[[#This Row],[Projectdependency 
-((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
-((low)1-(high)5)]]))/2</f>
-        <v>1.5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" t="s">
-        <v>6</v>
+      <c r="F26" t="s">
+        <v>61</v>
       </c>
       <c r="H26" t="s">
         <v>56</v>
@@ -2400,7 +2176,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -2409,16 +2185,19 @@
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2426,22 +2205,22 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="C28">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="H28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2449,91 +2228,262 @@
         <v>1</v>
       </c>
       <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
         <v>4</v>
       </c>
-      <c r="C29">
-        <f>(Tabelle1[[#This Row],[Projectdependency 
-((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
-((low)1-(high)5)]]))/2</f>
-        <v>1.5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" t="s">
-        <v>27</v>
+      <c r="F29" t="s">
+        <v>66</v>
       </c>
       <c r="H29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <f>(Tabelle1[[#This Row],[Projectdependency 
+((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
+((low)1-(high)5)]]))/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
         <v>2</v>
       </c>
-      <c r="B30">
+      <c r="B34">
         <v>5</v>
       </c>
-      <c r="C30">
+      <c r="C34">
         <f>(Tabelle1[[#This Row],[Projectdependency 
 ((low)1-(high)5)]]+(6-Tabelle1[[#This Row],[Effort 
 ((low)1-(high)5)]]))/2</f>
         <v>1.5</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
         <v>32</v>
       </c>
-      <c r="E30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" t="s">
-        <v>56</v>
-      </c>
+      <c r="H34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A2:H2">
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="67" priority="41">
       <formula>$H2="Deprecated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="22">
+    <cfRule type="expression" dxfId="66" priority="40">
       <formula>$H2="Implemented"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="21">
+    <cfRule type="expression" dxfId="65" priority="39">
       <formula>$H2="Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="64" priority="38">
       <formula>$H2="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="63" priority="37">
       <formula>$H2="Created"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="62" priority="31">
       <formula>$H2="InWork"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:H30">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="61" priority="20">
       <formula>$H3="Created"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="60" priority="21">
       <formula>$H3="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="59" priority="22">
       <formula>$H3="Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="58" priority="23">
       <formula>$H3="Implemented"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="57" priority="24">
       <formula>$H3="Deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:H30">
+    <cfRule type="expression" dxfId="56" priority="19">
+      <formula>$H3="InWork"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31:H32">
+    <cfRule type="expression" dxfId="53" priority="14">
+      <formula>$H31="Created"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="15">
+      <formula>$H31="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="16">
+      <formula>$H31="Ready"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="17">
+      <formula>$H31="Implemented"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="18">
+      <formula>$H31="Deprecated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31:H32">
+    <cfRule type="expression" dxfId="43" priority="13">
+      <formula>$H31="InWork"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:H33">
+    <cfRule type="expression" dxfId="41" priority="8">
+      <formula>$H31="Created"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="9">
+      <formula>$H31="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="10">
+      <formula>$H31="Ready"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="11">
+      <formula>$H31="Implemented"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="12">
+      <formula>$H31="Deprecated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:H33">
+    <cfRule type="expression" dxfId="31" priority="7">
+      <formula>$H31="InWork"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:H34">
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>$H34="Created"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>$H34="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>$H34="Ready"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>$H34="Implemented"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>$H34="Deprecated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:H34">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$H3="InWork"</formula>
+      <formula>$H34="InWork"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2543,7 +2493,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E3">
       <formula1>EmpList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H35">
       <formula1>statList</formula1>
     </dataValidation>
   </dataValidations>
@@ -2579,10 +2529,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2603,7 +2553,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -2615,7 +2565,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="8"/>
     </row>
@@ -2627,7 +2577,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -2639,7 +2589,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -2651,7 +2601,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -2663,16 +2613,16 @@
         <v>17</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>